<commit_message>
Addition of selection to library and pooled_sample viewsets and serializers. Addition of selection target to library list and selection information to sample detail. Addition of selection target to pool detail list.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v3_14_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v3_14_0.xlsx
@@ -9569,7 +9569,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9799,9 +9799,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1559160</xdr:colOff>
+      <xdr:colOff>1558800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9816,7 +9816,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="28440"/>
-          <a:ext cx="1482840" cy="542160"/>
+          <a:ext cx="1482480" cy="541800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>